<commit_message>
add something in tracker.xlsx
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Text Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F8D5A4-88C1-454A-B758-FB44B003D7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00806CCB-E072-4C64-987B-A4F37EA75072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Krish Naik" sheetId="1" r:id="rId1"/>
+    <sheet name="UnfoldDataScience" sheetId="2" r:id="rId2"/>
+    <sheet name="IndianAIProduction" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Playlist Titlle</t>
   </si>
@@ -75,9 +77,6 @@
     <t>https://www.youtube.com/playlist?list=PLZoTAELRMXVPwYGE2PXD3x0bfKnR0cJjN</t>
   </si>
   <si>
-    <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16</t>
-  </si>
-  <si>
     <t>MySQL Playlist</t>
   </si>
   <si>
@@ -124,13 +123,34 @@
   </si>
   <si>
     <t>https://www.youtube.com/playlist?list=PLZoTAELRMXVMhVyr3Ri9IQ-t5QPBtxzJO</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20</t>
+  </si>
+  <si>
+    <t>PlayList Title</t>
+  </si>
+  <si>
+    <t>Natural Language Processing Playlist</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLmPJQXJiMoUUSqSV7jcqGiiypGmQ_ogtb</t>
+  </si>
+  <si>
+    <t>Machine Learning and Deep Learning</t>
+  </si>
+  <si>
+    <t>Machine Learning And Deep Learning</t>
+  </si>
+  <si>
+    <t>1,2,3,4,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,8 +174,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +218,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,6 +250,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -485,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,128 +560,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
-        <v>16</v>
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>11</v>
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>151</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
-        <v>7</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>6</v>
@@ -627,42 +683,58 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="C15" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
@@ -695,21 +767,495 @@
       <c r="C25" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{ED09518C-45A0-43B1-8E60-9122400EEEA1}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{AFF8B50C-DB7E-40F3-8A11-738FBF7473A5}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{16ED1C7B-A14E-4096-B6DB-F0641C1E2DEB}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{1CF4D8DE-DBBF-46CB-82B1-88708C34619D}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{1E62C109-D385-4EC5-9CDD-A50D14C356E3}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{FD9998ED-4125-424C-AD2D-27E200A4A501}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{AFD08C97-CBB6-40F9-B2EA-2839F53E0F30}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{F0AD7323-957D-40AC-AC4A-4A416C28C60F}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{72769CE7-614F-4693-A1A5-D5A36AF9E12F}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{62C75D1A-25A4-4C9C-AEED-39973372DBFB}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{8E5FCB67-144A-469E-9C83-7F088E43FAFF}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{3E2A5EC8-0636-4312-90B1-E159B6C814CF}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{ED09518C-45A0-43B1-8E60-9122400EEEA1}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{AFF8B50C-DB7E-40F3-8A11-738FBF7473A5}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{16ED1C7B-A14E-4096-B6DB-F0641C1E2DEB}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{1CF4D8DE-DBBF-46CB-82B1-88708C34619D}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{1E62C109-D385-4EC5-9CDD-A50D14C356E3}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{FD9998ED-4125-424C-AD2D-27E200A4A501}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{AFD08C97-CBB6-40F9-B2EA-2839F53E0F30}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{F0AD7323-957D-40AC-AC4A-4A416C28C60F}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{72769CE7-614F-4693-A1A5-D5A36AF9E12F}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{62C75D1A-25A4-4C9C-AEED-39973372DBFB}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{8E5FCB67-144A-469E-9C83-7F088E43FAFF}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{3E2A5EC8-0636-4312-90B1-E159B6C814CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E1BAD9-978E-4A10-B8A2-F061C451F088}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{E6A9AD4B-6B52-47DA-A67B-B7B3B0BB5BEE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843FE81B-FB7C-4EA7-BF0A-DE16B1A445B8}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{BE5A960E-2215-4AEC-95B0-BC478827A57C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add some playlist in tracker
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Text Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00806CCB-E072-4C64-987B-A4F37EA75072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43390227-FE9E-4780-BFD1-11FF025CBFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Krish Naik" sheetId="1" r:id="rId1"/>
     <sheet name="UnfoldDataScience" sheetId="2" r:id="rId2"/>
     <sheet name="IndianAIProduction" sheetId="4" r:id="rId3"/>
+    <sheet name="CampuX" sheetId="5" r:id="rId4"/>
+    <sheet name="Murtaza's Workshop - Robotics" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t>Playlist Titlle</t>
   </si>
@@ -62,9 +64,6 @@
     <t>https://www.youtube.com/playlist?list=PLZoTAELRMXVMdJ5sqbCK2LiM0HhQVWNzm</t>
   </si>
   <si>
-    <t>1,2,3,4,5,6,7,8,9,10,11,20</t>
-  </si>
-  <si>
     <t>Complete Deep Learning</t>
   </si>
   <si>
@@ -125,9 +124,6 @@
     <t>https://www.youtube.com/playlist?list=PLZoTAELRMXVMhVyr3Ri9IQ-t5QPBtxzJO</t>
   </si>
   <si>
-    <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20</t>
-  </si>
-  <si>
     <t>PlayList Title</t>
   </si>
   <si>
@@ -143,7 +139,115 @@
     <t>Machine Learning And Deep Learning</t>
   </si>
   <si>
-    <t>1,2,3,4,</t>
+    <t>1 to 10,11,</t>
+  </si>
+  <si>
+    <t>1 to 20,</t>
+  </si>
+  <si>
+    <t>1 to 11,20</t>
+  </si>
+  <si>
+    <t>Machine Learning Metrics</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_RmvZJGOqRjqhOhTEmQW3vDdbQ</t>
+  </si>
+  <si>
+    <t>Regularization</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_RmvZuSEZ24Wlm13QpsfLlJBM4</t>
+  </si>
+  <si>
+    <t>Natural Language Processing(NLP)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_RmvZo7fp5kkIth6nRTeQQsjfX</t>
+  </si>
+  <si>
+    <t>100 Days of Deep Learning</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_RmvYuZauWaPlRTC54KxSNLtNn</t>
+  </si>
+  <si>
+    <t>Convolutional Neural Networks (CNNs)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_Rmvb6SAVpWjm0ZYPHo_KRXljU</t>
+  </si>
+  <si>
+    <t>Advance Statistics (ML Roadmap 2022)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_Rmvbe9wDJGXc28KKr6lp5Jn2g</t>
+  </si>
+  <si>
+    <t>100 Days of Machine Learning</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_Rmvbr7zKYQuBfsVkjoLcJgxHH</t>
+  </si>
+  <si>
+    <t>1,</t>
+  </si>
+  <si>
+    <t>Machine Learning Projects</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLKnIA16_RmvY5eP91BGPa0vXUYmIdtfPQ</t>
+  </si>
+  <si>
+    <t>OpenCV Python Tutorials for Beginners 2020</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,14</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r_sc0x7ndCsqdIkL7dwrmNF</t>
+  </si>
+  <si>
+    <t>Angle Finder OpenCV</t>
+  </si>
+  <si>
+    <t>Yolo v3 | OpenCV Python</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>Augmented Reality using OpenCV Python (2020)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r8vFXoAZPKyj-WLcD2aGoNZ</t>
+  </si>
+  <si>
+    <t>1 to 3</t>
+  </si>
+  <si>
+    <t>Advance Computer Vision</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r8nz4C5Yvd17KaXy8p0ufPH</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r-JNMQ0zJmv6SnXwgbA8JJp</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r9p7iYBg6z6tZP002DAJ41H</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r-7xWY3Oh2yOFp3EoxNOphH</t>
+  </si>
+  <si>
+    <t>3,</t>
+  </si>
+  <si>
+    <t>Computer Vision Projects</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r8jFS04rot-3NzidnV54Z2q</t>
   </si>
 </sst>
 </file>
@@ -238,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,16 +356,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -548,7 +656,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,20 +668,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -620,29 +728,29 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>16</v>
@@ -650,10 +758,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>11</v>
@@ -661,10 +769,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>151</v>
@@ -672,10 +780,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>6</v>
@@ -683,10 +791,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C11" s="2">
         <v>7</v>
@@ -694,10 +802,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="2">
         <v>6</v>
@@ -705,10 +813,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="C13" s="2">
         <v>8</v>
@@ -716,10 +824,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="C14" s="2">
         <v>5</v>
@@ -727,10 +835,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C15" s="2">
         <v>42</v>
@@ -793,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E1BAD9-978E-4A10-B8A2-F061C451F088}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,24 +914,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -840,16 +948,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -1031,36 +1139,36 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -1077,10 +1185,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2">
         <v>12</v>
@@ -1258,4 +1366,483 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E2F09C-1B3C-4616-A2B4-232FE8C2394F}">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="2">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{43E30678-C0FB-400E-939F-0C3478FB4F9F}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{C9CA59B9-CB12-4035-8E32-9A7D89CEEC24}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{BAB53A98-F328-4364-93DB-EC7A13A87011}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{7E91FDF3-55D8-4A15-920C-3CB060282388}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{B4FA20C7-A756-4DEA-A70D-D6C5FEE13B49}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{F0E5D832-94DD-4D2C-9232-9174E63F3D9A}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{55686960-B95B-4AA3-8B97-5606378DED5D}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{C549AAD4-3EA8-4897-8164-89ACC3189B42}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8645A614-CAED-4BD0-9C9A-DAD32DBD87CD}">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="2">
+        <v>33</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{6E22404C-5B86-44C5-A847-134B5AD0FACB}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{5BE94F4B-0031-486E-991D-ACAD5D234DDD}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{13C6318F-85FC-40B9-BB84-4BD38786EBEB}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{A03446D8-7A6A-4089-B83B-C15398AED3D9}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{4972216E-5032-4FE0-A8BC-7A9E7A31B423}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{0FD8DE1B-60E7-4EC4-AEAB-E89A7FE8B1FF}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{02C1AC40-DB16-44EC-984C-64716B475778}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add something on tracker
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Text Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43390227-FE9E-4780-BFD1-11FF025CBFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EFE237-C3A7-4EBB-A948-A10C082F8837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Krish Naik" sheetId="1" r:id="rId1"/>
@@ -145,9 +145,6 @@
     <t>1 to 20,</t>
   </si>
   <si>
-    <t>1 to 11,20</t>
-  </si>
-  <si>
     <t>Machine Learning Metrics</t>
   </si>
   <si>
@@ -248,6 +245,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/playlist?list=PLMoSUbG1Q_r8jFS04rot-3NzidnV54Z2q</t>
+  </si>
+  <si>
+    <t>1 to 15,20</t>
   </si>
 </sst>
 </file>
@@ -356,6 +356,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -366,10 +370,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,20 +668,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -728,7 +728,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -914,20 +914,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1151,20 +1151,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1372,7 +1372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E2F09C-1B3C-4616-A2B4-232FE8C2394F}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1386,20 +1386,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1420,25 +1420,25 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C5" s="2">
         <v>7</v>
@@ -1446,10 +1446,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
@@ -1457,10 +1457,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="C7" s="2">
         <v>28</v>
@@ -1468,10 +1468,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
@@ -1479,10 +1479,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C9" s="2">
         <v>7</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C10" s="2">
         <v>109</v>
@@ -1501,16 +1501,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C11" s="2">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1634,20 +1634,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1668,167 +1668,167 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="11"/>
+        <v>56</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="11"/>
+        <v>69</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="C10" s="2">
         <v>33</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="11"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="11"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="11"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="11"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="11"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="11"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="11"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="11"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="11"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="11"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="11"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="11"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="11"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="11"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="11"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="11"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="11"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="11"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="11"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="11"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="11"/>
+      <c r="E32" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add some krish naik hindi
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,28 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Text Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EFE237-C3A7-4EBB-A948-A10C082F8837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81E9975-2175-45D1-AA21-D66AB105B4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Krish Naik" sheetId="1" r:id="rId1"/>
-    <sheet name="UnfoldDataScience" sheetId="2" r:id="rId2"/>
-    <sheet name="IndianAIProduction" sheetId="4" r:id="rId3"/>
-    <sheet name="CampuX" sheetId="5" r:id="rId4"/>
-    <sheet name="Murtaza's Workshop - Robotics" sheetId="6" r:id="rId5"/>
+    <sheet name="Krish Naik Hindi" sheetId="7" r:id="rId2"/>
+    <sheet name="UnfoldDataScience" sheetId="2" r:id="rId3"/>
+    <sheet name="IndianAIProduction" sheetId="4" r:id="rId4"/>
+    <sheet name="CampuX" sheetId="5" r:id="rId5"/>
+    <sheet name="Murtaza's Workshop - Robotics" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
   <si>
     <t>Playlist Titlle</t>
   </si>
@@ -248,6 +257,15 @@
   </si>
   <si>
     <t>1 to 15,20</t>
+  </si>
+  <si>
+    <t>Machine Learning Playlist</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLTDARY42LDV7WGmlzZtY-w9pemyPrKNUZ</t>
+  </si>
+  <si>
+    <t>11,21,</t>
   </si>
 </sst>
 </file>
@@ -655,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,6 +916,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962DCF12-8601-4E71-892E-F40F360EA4C1}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{A1CAC83D-A5C8-4618-9B63-3F5D6B4874AF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E1BAD9-978E-4A10-B8A2-F061C451F088}">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -1134,7 +1283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843FE81B-FB7C-4EA7-BF0A-DE16B1A445B8}">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -1368,7 +1517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E2F09C-1B3C-4616-A2B4-232FE8C2394F}">
   <dimension ref="A1:E32"/>
   <sheetViews>
@@ -1616,7 +1765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8645A614-CAED-4BD0-9C9A-DAD32DBD87CD}">
   <dimension ref="A1:E32"/>
   <sheetViews>

</xml_diff>

<commit_message>
add some databse source name
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Text Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47ACACB-60A3-4B24-8AEE-299AC7335B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF9A633-9ED5-42BB-ABD3-2A8FF45FB00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1581,7 +1581,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>